<commit_message>
Complete version of random GA with levenshtain path penalty. Also a backup before replacing the penalty function and run grid search again.
</commit_message>
<xml_diff>
--- a/Evaluation result/Initialization values final 01_29.xlsx
+++ b/Evaluation result/Initialization values final 01_29.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/Dropbox/City Tourism Estimation/Evaluation result/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UserName\Dropbox\City Tourism Estimation\Evaluation result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3EEFAE2-D966-0F44-88B7-621DF7511D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="60" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="375" yWindow="60" windowWidth="28035" windowHeight="17445"/>
   </bookViews>
   <sheets>
     <sheet name="Initialization values final 01_" sheetId="1" r:id="rId1"/>
@@ -46,26 +45,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="游ゴシック Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -73,7 +72,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -81,7 +80,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -89,35 +88,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -125,7 +124,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -133,14 +132,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -148,14 +147,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -163,7 +162,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -171,15 +170,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -529,48 +535,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - アクセント 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - アクセント 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - アクセント 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="アクセント 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="アクセント 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="アクセント 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="アクセント 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="アクセント 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="アクセント 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="タイトル" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="チェック セル" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="どちらでもない" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="メモ" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="リンク セル" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="出力" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="悪い" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="集計" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="計算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="見出し 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="見出し 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="見出し 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="見出し 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="警告文" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="良い" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="入力" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="説明文" xfId="16" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -588,8 +594,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G43" totalsRowShown="0">
   <autoFilter ref="A1:G43"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G43">
-    <sortCondition ref="A1:A43"/>
+  <sortState ref="A2:G43">
+    <sortCondition ref="F1:F43"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="index"/>
@@ -903,13 +909,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -932,122 +938,122 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>3.0956271E-2</v>
+        <v>2.7327872E-2</v>
       </c>
       <c r="C2">
-        <v>296.84482789999998</v>
+        <v>327.96060699999998</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>2399.6330589999998</v>
+        <v>1832.2683959999999</v>
       </c>
       <c r="G2" s="1">
-        <v>2495190000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>549817000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>3.2656722999999999E-2</v>
+        <v>2.9567533E-2</v>
       </c>
       <c r="C3">
-        <v>330.54134579999999</v>
+        <v>308.5271017</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F3">
-        <v>2301.669535</v>
+        <v>1861.2265050000001</v>
       </c>
       <c r="G3" s="1">
-        <v>5743020000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>401805000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>2.5426958E-2</v>
+        <v>3.2639538000000003E-2</v>
       </c>
       <c r="C4">
-        <v>339.69295199999999</v>
+        <v>290.60189919999999</v>
       </c>
       <c r="D4">
         <v>0.1</v>
       </c>
       <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1879.276901</v>
+      </c>
+      <c r="G4" s="1">
+        <v>331272000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>3.8089451000000003E-2</v>
+      </c>
+      <c r="C5">
+        <v>275.6908689</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
         <v>0.6</v>
       </c>
-      <c r="F4">
-        <v>2311.041436</v>
-      </c>
-      <c r="G4" s="1">
-        <v>5294750000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>3.7889539E-2</v>
-      </c>
-      <c r="C5">
-        <v>240.72747010000001</v>
-      </c>
-      <c r="D5">
-        <v>0.1</v>
-      </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
       <c r="F5">
-        <v>2285.3840300000002</v>
+        <v>1911.5644259999999</v>
       </c>
       <c r="G5" s="1">
-        <v>6619360000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>235625000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B6">
-        <v>2.8319179999999999E-2</v>
+        <v>2.1121289000000001E-2</v>
       </c>
       <c r="C6">
-        <v>296.93426770000002</v>
+        <v>270.40360170000002</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F6">
-        <v>2249.4101580000001</v>
+        <v>1943.8975740000001</v>
       </c>
       <c r="G6" s="1">
-        <v>9091320000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>168474000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1070,812 +1076,812 @@
         <v>82325700000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>3.2639538000000003E-2</v>
+        <v>2.5555114E-2</v>
       </c>
       <c r="C8">
-        <v>290.60189919999999</v>
+        <v>326.35920279999999</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
-        <v>1879.276901</v>
+        <v>2036.2196530000001</v>
       </c>
       <c r="G8" s="1">
-        <v>331272000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>66605100000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>2.9028282999999998E-2</v>
+        <v>4.4918918000000002E-2</v>
       </c>
       <c r="C9">
-        <v>317.20581800000002</v>
+        <v>321.16298169999999</v>
       </c>
       <c r="D9">
         <v>0.5</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>2119.6304850000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>29839900000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>2.8453345000000001E-2</v>
+      </c>
+      <c r="C10">
+        <v>279.09614720000002</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.6</v>
+      </c>
+      <c r="F10">
+        <v>2174.9946439999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>17817100000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2.4612367E-2</v>
+      </c>
+      <c r="C11">
+        <v>316.17229279999998</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>0.2</v>
       </c>
-      <c r="F9">
-        <v>2297.5035050000001</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5954930000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>2.5555114E-2</v>
-      </c>
-      <c r="C10">
-        <v>326.35920279999999</v>
-      </c>
-      <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <v>0.4</v>
-      </c>
-      <c r="F10">
-        <v>2036.2196530000001</v>
-      </c>
-      <c r="G10" s="1">
-        <v>66605100000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>3.8089451000000003E-2</v>
-      </c>
-      <c r="C11">
-        <v>275.6908689</v>
-      </c>
-      <c r="D11">
-        <v>0.5</v>
-      </c>
-      <c r="E11">
-        <v>0.6</v>
-      </c>
       <c r="F11">
-        <v>1911.5644259999999</v>
+        <v>2178.322228</v>
       </c>
       <c r="G11" s="1">
-        <v>235625000000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17280500000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>2.9567533E-2</v>
+        <v>2.8319179999999999E-2</v>
       </c>
       <c r="C12">
-        <v>308.5271017</v>
+        <v>296.93426770000002</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2249.4101580000001</v>
+      </c>
+      <c r="G12" s="1">
+        <v>9091320000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3.7889539E-2</v>
+      </c>
+      <c r="C13">
+        <v>240.72747010000001</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
         <v>0.8</v>
       </c>
-      <c r="F12">
-        <v>1861.2265050000001</v>
-      </c>
-      <c r="G12" s="1">
-        <v>401805000000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>4.4918918000000002E-2</v>
-      </c>
-      <c r="C13">
-        <v>321.16298169999999</v>
-      </c>
-      <c r="D13">
-        <v>0.5</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="F13">
-        <v>2119.6304850000001</v>
+        <v>2285.3840300000002</v>
       </c>
       <c r="G13" s="1">
-        <v>29839900000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6619360000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>2.6426384000000001E-2</v>
+        <v>2.9028282999999998E-2</v>
       </c>
       <c r="C14">
-        <v>276.85142189999999</v>
+        <v>317.20581800000002</v>
       </c>
       <c r="D14">
         <v>0.5</v>
       </c>
       <c r="E14">
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>2297.5035050000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5954930000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3.2656722999999999E-2</v>
+      </c>
+      <c r="C15">
+        <v>330.54134579999999</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="E15">
+        <v>0.4</v>
+      </c>
+      <c r="F15">
+        <v>2301.669535</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5743020000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>3158.175812</v>
-      </c>
-      <c r="G14">
-        <v>10262990809</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>3.4916750000000003E-2</v>
-      </c>
-      <c r="C15">
-        <v>349.3158919</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15">
+      <c r="B16">
+        <v>2.5426958E-2</v>
+      </c>
+      <c r="C16">
+        <v>339.69295199999999</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="E16">
+        <v>0.6</v>
+      </c>
+      <c r="F16">
+        <v>2311.041436</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5294750000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>3.0956271E-2</v>
+      </c>
+      <c r="C17">
+        <v>296.84482789999998</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>0.2</v>
+      </c>
+      <c r="F17">
+        <v>2399.6330589999998</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2495190000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>2.7103558999999999E-2</v>
+      </c>
+      <c r="C18">
+        <v>340.35148989999999</v>
+      </c>
+      <c r="D18">
         <v>5</v>
       </c>
-      <c r="F15">
-        <v>4224.534842</v>
-      </c>
-      <c r="G15">
-        <v>30508585.640000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>2.4612367E-2</v>
-      </c>
-      <c r="C16">
-        <v>316.17229279999998</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+      <c r="E18">
         <v>0.2</v>
       </c>
-      <c r="F16">
-        <v>2178.322228</v>
-      </c>
-      <c r="G16" s="1">
-        <v>17280500000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>2.7327872E-2</v>
-      </c>
-      <c r="C17">
-        <v>327.96060699999998</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
+      <c r="F18">
+        <v>2639.0348509999999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>372475000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>2.0579732999999999E-2</v>
+      </c>
+      <c r="C19">
+        <v>348.58488979999998</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
         <v>0.4</v>
       </c>
-      <c r="F17">
-        <v>1832.2683959999999</v>
-      </c>
-      <c r="G17" s="1">
-        <v>549817000000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>2.8453345000000001E-2</v>
-      </c>
-      <c r="C18">
-        <v>279.09614720000002</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
+      <c r="F19">
+        <v>2805.4921880000002</v>
+      </c>
+      <c r="G19" s="1">
+        <v>109602000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>2.5765855000000001E-2</v>
+      </c>
+      <c r="C20">
+        <v>312.3820197</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>2830.20804</v>
+      </c>
+      <c r="G20">
+        <v>91967163910</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>2.7723620000000001E-2</v>
+      </c>
+      <c r="C21">
+        <v>287.6551379</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>0.6</v>
       </c>
-      <c r="F18">
-        <v>2174.9946439999999</v>
-      </c>
-      <c r="G18" s="1">
-        <v>17817100000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>2.6277228999999999E-2</v>
-      </c>
-      <c r="C19">
-        <v>385.17780909999999</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0.8</v>
-      </c>
-      <c r="F19">
-        <v>3154.4719009999999</v>
-      </c>
-      <c r="G19">
-        <v>10506709773</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="F21">
+        <v>3043.903941</v>
+      </c>
+      <c r="G21">
+        <v>21447720562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A22">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B22">
         <v>2.5495422E-2</v>
       </c>
-      <c r="C20">
+      <c r="C22">
         <v>301.11587889999998</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>3135.4061190000002</v>
-      </c>
-      <c r="G20">
-        <v>11861072736</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>3.2037777000000003E-2</v>
-      </c>
-      <c r="C21">
-        <v>307.35027580000002</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21">
-        <v>3541.3663959999999</v>
-      </c>
-      <c r="G21">
-        <v>1038921564</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>3.8914994000000001E-2</v>
-      </c>
-      <c r="C22">
-        <v>341.25440759999998</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>4609.948515</v>
+        <v>3135.4061190000002</v>
       </c>
       <c r="G22">
-        <v>5322044.4570000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11861072736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>2.1121289000000001E-2</v>
+        <v>2.6277228999999999E-2</v>
       </c>
       <c r="C23">
-        <v>270.40360170000002</v>
+        <v>385.17780909999999</v>
       </c>
       <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0.8</v>
+      </c>
+      <c r="F23">
+        <v>3154.4719009999999</v>
+      </c>
+      <c r="G23">
+        <v>10506709773</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>2.6426384000000001E-2</v>
+      </c>
+      <c r="C24">
+        <v>276.85142189999999</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
         <v>2</v>
       </c>
-      <c r="E23">
-        <v>0.2</v>
-      </c>
-      <c r="F23">
-        <v>1943.8975740000001</v>
-      </c>
-      <c r="G23" s="1">
-        <v>168474000000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>2.0579732999999999E-2</v>
-      </c>
-      <c r="C24">
-        <v>348.58488979999998</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <v>0.4</v>
-      </c>
       <c r="F24">
-        <v>2805.4921880000002</v>
-      </c>
-      <c r="G24" s="1">
-        <v>109602000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3158.175812</v>
+      </c>
+      <c r="G24">
+        <v>10262990809</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>2.7723620000000001E-2</v>
+        <v>2.7885448E-2</v>
       </c>
       <c r="C25">
-        <v>287.6551379</v>
+        <v>305.83077639999999</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25">
+        <v>0.8</v>
+      </c>
+      <c r="F25">
+        <v>3208.8329010000002</v>
+      </c>
+      <c r="G25">
+        <v>7465483869</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>2.6810549999999999E-2</v>
+      </c>
+      <c r="C26">
+        <v>289.24257130000001</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>0.4</v>
+      </c>
+      <c r="F26">
+        <v>3224.8895149999998</v>
+      </c>
+      <c r="G26">
+        <v>6756210858</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>3.0382052999999999E-2</v>
+      </c>
+      <c r="C27">
+        <v>302.43500540000002</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>0.4</v>
+      </c>
+      <c r="F27">
+        <v>3453.685446</v>
+      </c>
+      <c r="G27">
+        <v>1715317001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>2.2989701000000001E-2</v>
+      </c>
+      <c r="C28">
+        <v>240.36880579999999</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28">
         <v>0.6</v>
       </c>
-      <c r="F25">
-        <v>3043.903941</v>
-      </c>
-      <c r="G25">
-        <v>21447720562</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>2.7885448E-2</v>
-      </c>
-      <c r="C26">
-        <v>305.83077639999999</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>0.8</v>
-      </c>
-      <c r="F26">
-        <v>3208.8329010000002</v>
-      </c>
-      <c r="G26">
-        <v>7465483869</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="F28">
+        <v>3457.6910790000002</v>
+      </c>
+      <c r="G28">
+        <v>1676008476</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>3.4719856E-2</v>
       </c>
-      <c r="C27">
+      <c r="C29">
         <v>305.82309229999998</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>3468.2744459999999</v>
-      </c>
-      <c r="G27">
-        <v>1576633971</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>1.8538733000000002E-2</v>
-      </c>
-      <c r="C28">
-        <v>281.45250399999998</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <v>4276.8612480000002</v>
-      </c>
-      <c r="G28">
-        <v>23850461.289999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>3.7333782000000003E-2</v>
-      </c>
-      <c r="C29">
-        <v>287.5110123</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>5400.7437030000001</v>
+        <v>3468.2744459999999</v>
       </c>
       <c r="G29">
-        <v>224351.32620000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1576633971</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B30">
-        <v>2.7103558999999999E-2</v>
+        <v>3.2037777000000003E-2</v>
       </c>
       <c r="C30">
-        <v>340.35148989999999</v>
+        <v>307.35027580000002</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>2639.0348509999999</v>
-      </c>
-      <c r="G30" s="1">
-        <v>372475000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3541.3663959999999</v>
+      </c>
+      <c r="G30">
+        <v>1038921564</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>2.6810549999999999E-2</v>
+        <v>3.3389733999999997E-2</v>
       </c>
       <c r="C31">
-        <v>289.24257130000001</v>
+        <v>305.52425149999999</v>
       </c>
       <c r="D31">
         <v>5</v>
       </c>
       <c r="E31">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="F31">
-        <v>3224.8895149999998</v>
+        <v>4032.044594</v>
       </c>
       <c r="G31">
-        <v>6756210858</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>77534227.739999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B32">
-        <v>2.2989701000000001E-2</v>
+        <v>2.1836735999999999E-2</v>
       </c>
       <c r="C32">
-        <v>240.36880579999999</v>
+        <v>380.08856989999998</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E32">
         <v>0.6</v>
       </c>
       <c r="F32">
-        <v>3457.6910790000002</v>
+        <v>4149.389416</v>
       </c>
       <c r="G32">
-        <v>1676008476</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>43683366.829999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B33">
-        <v>3.3389733999999997E-2</v>
+        <v>3.4916750000000003E-2</v>
       </c>
       <c r="C33">
-        <v>305.52425149999999</v>
+        <v>349.3158919</v>
       </c>
       <c r="D33">
+        <v>0.5</v>
+      </c>
+      <c r="E33">
         <v>5</v>
       </c>
-      <c r="E33">
-        <v>0.8</v>
-      </c>
       <c r="F33">
-        <v>4032.044594</v>
+        <v>4224.534842</v>
       </c>
       <c r="G33">
-        <v>77534227.739999995</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>30508585.640000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>1.8538733000000002E-2</v>
+      </c>
+      <c r="C34">
+        <v>281.45250399999998</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>4276.8612480000002</v>
+      </c>
+      <c r="G34">
+        <v>23850461.289999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A35">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>2.9226392E-2</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>310.99428879999999</v>
-      </c>
-      <c r="D34">
-        <v>5</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>4301.2229310000002</v>
-      </c>
-      <c r="G34">
-        <v>21289278.879999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>2.5284852E-2</v>
-      </c>
-      <c r="C35">
-        <v>328.43203970000002</v>
       </c>
       <c r="D35">
         <v>5</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>5400.7172769999997</v>
+        <v>4301.2229310000002</v>
       </c>
       <c r="G35">
-        <v>224373.28229999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21289278.879999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B36">
-        <v>2.4614860999999998E-2</v>
+        <v>2.6999076E-2</v>
       </c>
       <c r="C36">
-        <v>302.0089557</v>
+        <v>363.46029609999999</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>0.8</v>
       </c>
       <c r="F36">
-        <v>6164.4865049999999</v>
+        <v>4445.6517329999997</v>
       </c>
       <c r="G36">
-        <v>15924.355939999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10997431.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B37">
-        <v>2.5765855000000001E-2</v>
+        <v>2.3076042000000001E-2</v>
       </c>
       <c r="C37">
-        <v>312.3820197</v>
+        <v>298.92506020000002</v>
       </c>
       <c r="D37">
         <v>7</v>
       </c>
       <c r="E37">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>2830.20804</v>
+        <v>4510.9906929999997</v>
       </c>
       <c r="G37">
-        <v>91967163910</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8214126.3420000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B38">
-        <v>3.0382052999999999E-2</v>
+        <v>3.8914994000000001E-2</v>
       </c>
       <c r="C38">
-        <v>302.43500540000002</v>
+        <v>341.25440759999998</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0.4</v>
+        <v>5</v>
       </c>
       <c r="F38">
-        <v>3453.685446</v>
+        <v>4609.948515</v>
       </c>
       <c r="G38">
-        <v>1715317001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5322044.4570000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39">
-        <v>2.1836735999999999E-2</v>
+        <v>2.5284852E-2</v>
       </c>
       <c r="C39">
-        <v>380.08856989999998</v>
+        <v>328.43203970000002</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>4149.389416</v>
+        <v>5400.7172769999997</v>
       </c>
       <c r="G39">
-        <v>43683366.829999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224373.28229999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B40">
-        <v>2.6999076E-2</v>
+        <v>3.7333782000000003E-2</v>
       </c>
       <c r="C40">
-        <v>363.46029609999999</v>
+        <v>287.5110123</v>
       </c>
       <c r="D40">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>0.8</v>
+        <v>5</v>
       </c>
       <c r="F40">
-        <v>4445.6517329999997</v>
+        <v>5400.7437030000001</v>
       </c>
       <c r="G40">
-        <v>10997431.08</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>224351.32620000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <v>2.3076042000000001E-2</v>
+        <v>2.7264643000000002E-2</v>
       </c>
       <c r="C41">
-        <v>298.92506020000002</v>
+        <v>344.80450530000002</v>
       </c>
       <c r="D41">
         <v>7</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>4510.9906929999997</v>
+        <v>5845.7351289999997</v>
       </c>
       <c r="G41">
-        <v>8214126.3420000002</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>46048.695299999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B42">
-        <v>2.7264643000000002E-2</v>
+        <v>2.4614860999999998E-2</v>
       </c>
       <c r="C42">
-        <v>344.80450530000002</v>
+        <v>302.0089557</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>5845.7351289999997</v>
+        <v>6164.4865049999999</v>
       </c>
       <c r="G42">
-        <v>46048.695299999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>15924.355939999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>41</v>
       </c>
@@ -1899,6 +1905,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>